<commit_message>
Updated the Time Sheet 08/16/2021
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -105,32 +105,25 @@
     <t xml:space="preserve">4hr 00min</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">* Explored the alternative of FileBrowse
+    <t xml:space="preserve">* Explored the alternative of FileBrowse
 * Migrated the FileBrowse library to tkinter.filedialog.askopenfile
 * Migrated the String library to str
 * Setup EPICS in local machine
 * Tried running the app in python 2.7 environment
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
 In-Progress
  * Learning basics of epics and tkinter (GUI)  libraries</t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">7hr 00min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Handled the PV connection status errors
+* Started Working on Task 2
+* Setup musclex project in my local system
+* Running musclex
+* Going through the musclex Documentation
+In-Progress
+  * Analyse the code for Task 2.1</t>
   </si>
 </sst>
 </file>
@@ -323,11 +316,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,10 +448,10 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="71.3"/>
@@ -522,19 +515,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+    <row r="5" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B5" s="9" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
@@ -6569,12 +6576,15 @@
       <c r="D1000" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated the time sheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -567,10 +567,10 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="71.3"/>
@@ -868,7 +868,7 @@
         <v>1.75</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>23</v>

</xml_diff>